<commit_message>
PCS WIP with payback
</commit_message>
<xml_diff>
--- a/Inputs/InputSchedule.xlsx
+++ b/Inputs/InputSchedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/ah17992_bristol_ac_uk/Documents/DP5/Shared/DP5_modelling/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:4000b_{DEB44F97-88D2-433A-B317-5E3E680ACB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72EAFE30-A94F-4A73-B468-296C8038DCCB}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="13_ncr:4000b_{DEB44F97-88D2-433A-B317-5E3E680ACB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69EBE43E-59F8-480A-B057-375AA2A6573F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="71">
   <si>
     <t>Case</t>
   </si>
@@ -206,13 +206,43 @@
     <t>Electric Heater</t>
   </si>
   <si>
-    <t>Fixed Tariff</t>
-  </si>
-  <si>
     <t>Fixed22Tariff.csv</t>
   </si>
   <si>
     <t>Number</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Current Household of 4</t>
+  </si>
+  <si>
+    <t>Costs</t>
+  </si>
+  <si>
+    <t>Cost of Change</t>
+  </si>
+  <si>
+    <t>Current Household of 5</t>
+  </si>
+  <si>
+    <t>Current Household of 6</t>
+  </si>
+  <si>
+    <t>Current Household of 7</t>
+  </si>
+  <si>
+    <t>Current Household of 8</t>
+  </si>
+  <si>
+    <t>Current Household of 9</t>
+  </si>
+  <si>
+    <t>Agile Tariff</t>
+  </si>
+  <si>
+    <t>Fourth</t>
   </si>
 </sst>
 </file>
@@ -707,7 +737,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -718,6 +748,12 @@
       <alignment textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="25" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="36" applyAlignment="1">
       <alignment textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -765,7 +801,52 @@
     <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1083,951 +1164,1291 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AV7"/>
+  <dimension ref="A1:AY9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T22" sqref="T22"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="3.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="3.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="34" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="36" max="40" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="42" width="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="44" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="4" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="4" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="37" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="39" max="43" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="45" width="5" bestFit="1" customWidth="1"/>
+    <col min="46" max="47" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="4" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="4" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" s="5" customFormat="1" ht="111" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" s="5" customFormat="1" ht="121.5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="Q1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AG1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AI1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AK1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AM1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="AN1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AO1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AP1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="AQ1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AR1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" s="5" t="s">
+      <c r="AS1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" s="5" t="s">
+      <c r="AT1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AR1" s="5" t="s">
+      <c r="AU1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AS1" s="5" t="s">
+      <c r="AV1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" s="5" t="s">
+      <c r="AW1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AU1" s="5" t="s">
+      <c r="AX1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" s="5" t="s">
+      <c r="AY1" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>54</v>
       </c>
-      <c r="D2">
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="G2">
         <v>54</v>
       </c>
-      <c r="E2">
+      <c r="H2">
         <v>13700</v>
       </c>
-      <c r="F2">
+      <c r="I2">
         <v>2437.5</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
         <v>0.15</v>
       </c>
-      <c r="I2">
+      <c r="L2">
         <v>0.9</v>
       </c>
-      <c r="J2">
+      <c r="M2">
         <v>7.4</v>
       </c>
-      <c r="K2">
+      <c r="N2">
         <v>0.9</v>
       </c>
-      <c r="M2" t="s">
-        <v>47</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q2" t="s">
         <v>48</v>
       </c>
-      <c r="O2">
+      <c r="R2">
         <v>4</v>
       </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="R2">
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="U2">
         <v>0.2</v>
       </c>
-      <c r="S2" s="1">
+      <c r="V2" s="1">
         <v>43521.791666666664</v>
       </c>
-      <c r="T2" s="1">
+      <c r="W2" s="1">
         <v>43524.291666666664</v>
       </c>
-      <c r="U2" t="s">
+      <c r="X2" t="s">
         <v>49</v>
       </c>
-      <c r="V2" t="s">
+      <c r="Y2" t="s">
         <v>50</v>
       </c>
-      <c r="X2" t="s">
+      <c r="AA2" t="s">
         <v>51</v>
       </c>
-      <c r="Y2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD2" t="s">
         <v>56</v>
       </c>
-      <c r="AB2">
+      <c r="AE2">
         <v>9</v>
       </c>
-      <c r="AC2">
+      <c r="AF2">
         <v>0.8</v>
       </c>
-      <c r="AD2">
+      <c r="AG2">
         <v>0</v>
       </c>
-      <c r="AF2">
-        <v>1</v>
-      </c>
-      <c r="AG2">
+      <c r="AI2">
+        <v>1</v>
+      </c>
+      <c r="AJ2">
         <v>5</v>
       </c>
-      <c r="AH2">
+      <c r="AK2">
         <v>6</v>
       </c>
-      <c r="AJ2">
+      <c r="AM2">
         <v>10</v>
       </c>
-      <c r="AK2">
+      <c r="AN2">
         <v>2</v>
       </c>
-      <c r="AL2">
+      <c r="AO2">
         <v>10</v>
       </c>
-      <c r="AM2">
+      <c r="AP2">
         <v>15</v>
       </c>
-      <c r="AN2">
+      <c r="AQ2">
         <v>21</v>
       </c>
-      <c r="AO2">
+      <c r="AR2">
         <v>2000</v>
       </c>
-      <c r="AP2">
+      <c r="AS2">
         <v>2000</v>
       </c>
-      <c r="AQ2">
-        <v>1</v>
-      </c>
-      <c r="AR2">
+      <c r="AT2">
+        <v>1</v>
+      </c>
+      <c r="AU2">
         <v>40</v>
       </c>
-      <c r="AS2">
+      <c r="AV2">
         <v>120</v>
       </c>
-      <c r="AT2">
+      <c r="AW2">
         <v>40</v>
       </c>
-      <c r="AU2">
+      <c r="AX2">
         <v>0.3</v>
       </c>
-      <c r="AV2">
+      <c r="AY2">
         <v>0.16</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>54</v>
       </c>
-      <c r="D3">
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="G3">
         <v>54</v>
       </c>
-      <c r="E3">
+      <c r="H3">
         <v>13700</v>
       </c>
-      <c r="F3">
+      <c r="I3">
         <v>2437.5</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
         <v>0.15</v>
       </c>
-      <c r="I3">
+      <c r="L3">
         <v>0.9</v>
       </c>
-      <c r="J3">
+      <c r="M3">
         <v>7.4</v>
       </c>
-      <c r="K3">
+      <c r="N3">
         <v>0.9</v>
       </c>
-      <c r="M3" t="s">
-        <v>47</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="P3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q3" t="s">
         <v>48</v>
       </c>
-      <c r="O3">
+      <c r="R3">
         <v>4</v>
       </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="R3">
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="U3">
         <v>0.2</v>
       </c>
-      <c r="S3" s="1">
+      <c r="V3" s="1">
         <v>43521.791666666664</v>
       </c>
-      <c r="T3" s="1">
+      <c r="W3" s="1">
         <v>43524.291666666664</v>
       </c>
-      <c r="U3" t="s">
+      <c r="X3" t="s">
         <v>49</v>
       </c>
-      <c r="V3" t="s">
+      <c r="Y3" t="s">
         <v>50</v>
       </c>
-      <c r="X3" t="s">
+      <c r="AA3" t="s">
         <v>51</v>
       </c>
-      <c r="Y3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD3" t="s">
         <v>56</v>
       </c>
-      <c r="AB3">
+      <c r="AE3">
         <v>9</v>
       </c>
-      <c r="AC3">
+      <c r="AF3">
         <v>0.8</v>
       </c>
-      <c r="AD3">
-        <v>1</v>
-      </c>
-      <c r="AF3">
-        <v>1</v>
-      </c>
       <c r="AG3">
+        <v>1</v>
+      </c>
+      <c r="AI3">
+        <v>1</v>
+      </c>
+      <c r="AJ3">
         <v>5</v>
       </c>
-      <c r="AH3">
+      <c r="AK3">
         <v>6</v>
       </c>
-      <c r="AJ3">
+      <c r="AM3">
         <v>10</v>
       </c>
-      <c r="AK3">
+      <c r="AN3">
         <v>2</v>
       </c>
-      <c r="AL3">
+      <c r="AO3">
         <v>10</v>
       </c>
-      <c r="AM3">
+      <c r="AP3">
         <v>15</v>
       </c>
-      <c r="AN3">
+      <c r="AQ3">
         <v>21</v>
       </c>
-      <c r="AO3">
+      <c r="AR3">
         <v>2000</v>
       </c>
-      <c r="AP3">
+      <c r="AS3">
         <v>2000</v>
       </c>
-      <c r="AQ3">
-        <v>1</v>
-      </c>
-      <c r="AR3">
+      <c r="AT3">
+        <v>1</v>
+      </c>
+      <c r="AU3">
         <v>40</v>
       </c>
-      <c r="AS3">
+      <c r="AV3">
         <v>120</v>
       </c>
-      <c r="AT3">
+      <c r="AW3">
         <v>40</v>
       </c>
-      <c r="AU3">
+      <c r="AX3">
         <v>0.3</v>
       </c>
-      <c r="AV3">
+      <c r="AY3">
         <v>0.16</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>57</v>
       </c>
-      <c r="D4">
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4">
+        <v>10000</v>
+      </c>
+      <c r="G4">
         <v>54</v>
       </c>
-      <c r="E4">
+      <c r="H4">
         <v>13700</v>
       </c>
-      <c r="F4">
+      <c r="I4">
         <v>2437.5</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
         <v>0.15</v>
       </c>
-      <c r="I4">
+      <c r="L4">
         <v>0.9</v>
       </c>
-      <c r="J4">
+      <c r="M4">
         <v>7.4</v>
       </c>
-      <c r="K4">
+      <c r="N4">
         <v>0.9</v>
       </c>
-      <c r="M4" t="s">
-        <v>47</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q4" t="s">
         <v>48</v>
       </c>
-      <c r="O4">
+      <c r="R4">
         <v>4</v>
       </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="R4">
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="U4">
         <v>0.2</v>
       </c>
-      <c r="S4" s="1">
+      <c r="V4" s="1">
         <v>43521.791666666664</v>
       </c>
-      <c r="T4" s="1">
+      <c r="W4" s="1">
         <v>43524.291666666664</v>
       </c>
-      <c r="U4" t="s">
+      <c r="X4" t="s">
         <v>49</v>
       </c>
-      <c r="V4" t="s">
+      <c r="Y4" t="s">
         <v>50</v>
       </c>
-      <c r="X4" t="s">
+      <c r="AA4" t="s">
         <v>51</v>
       </c>
-      <c r="Y4" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD4" t="s">
         <v>53</v>
       </c>
-      <c r="AB4">
+      <c r="AE4">
         <v>9</v>
       </c>
-      <c r="AC4">
+      <c r="AF4">
         <v>0.8</v>
       </c>
-      <c r="AD4">
+      <c r="AG4">
         <v>0</v>
       </c>
-      <c r="AF4">
-        <v>1</v>
-      </c>
-      <c r="AG4">
+      <c r="AI4">
+        <v>1</v>
+      </c>
+      <c r="AJ4">
         <v>5</v>
       </c>
-      <c r="AH4">
+      <c r="AK4">
         <v>6</v>
       </c>
-      <c r="AJ4">
+      <c r="AM4">
         <v>10</v>
       </c>
-      <c r="AK4">
+      <c r="AN4">
         <v>2</v>
       </c>
-      <c r="AL4">
+      <c r="AO4">
         <v>10</v>
       </c>
-      <c r="AM4">
+      <c r="AP4">
         <v>15</v>
       </c>
-      <c r="AN4">
+      <c r="AQ4">
         <v>21</v>
       </c>
-      <c r="AO4">
+      <c r="AR4">
         <v>2000</v>
       </c>
-      <c r="AP4">
+      <c r="AS4">
         <v>2000</v>
       </c>
-      <c r="AQ4">
-        <v>1</v>
-      </c>
-      <c r="AR4">
+      <c r="AT4">
+        <v>1</v>
+      </c>
+      <c r="AU4">
         <v>40</v>
       </c>
-      <c r="AS4">
+      <c r="AV4">
         <v>120</v>
       </c>
-      <c r="AT4">
+      <c r="AW4">
         <v>40</v>
       </c>
-      <c r="AU4">
+      <c r="AX4">
         <v>0.3</v>
       </c>
-      <c r="AV4">
+      <c r="AY4">
         <v>0.16</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>57</v>
       </c>
-      <c r="D5">
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5">
+        <v>10000</v>
+      </c>
+      <c r="G5">
         <v>54</v>
       </c>
-      <c r="E5">
+      <c r="H5">
         <v>13700</v>
       </c>
-      <c r="F5">
+      <c r="I5">
         <v>2437.5</v>
       </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
         <v>0.15</v>
       </c>
-      <c r="I5">
+      <c r="L5">
         <v>0.9</v>
       </c>
-      <c r="J5">
+      <c r="M5">
         <v>7.4</v>
       </c>
-      <c r="K5">
+      <c r="N5">
         <v>0.9</v>
       </c>
-      <c r="M5" t="s">
-        <v>47</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="P5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q5" t="s">
         <v>48</v>
       </c>
-      <c r="O5">
+      <c r="R5">
         <v>4</v>
       </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-      <c r="R5">
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="U5">
         <v>0.2</v>
       </c>
-      <c r="S5" s="1">
+      <c r="V5" s="1">
         <v>43521.791666666664</v>
       </c>
-      <c r="T5" s="1">
+      <c r="W5" s="1">
         <v>43524.291666666664</v>
       </c>
-      <c r="U5" t="s">
+      <c r="X5" t="s">
         <v>49</v>
       </c>
-      <c r="V5" t="s">
+      <c r="Y5" t="s">
         <v>50</v>
       </c>
-      <c r="X5" t="s">
+      <c r="AA5" t="s">
         <v>51</v>
       </c>
-      <c r="Y5" t="s">
-        <v>55</v>
-      </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD5" t="s">
         <v>53</v>
       </c>
-      <c r="AB5">
+      <c r="AE5">
         <v>9</v>
       </c>
-      <c r="AC5">
+      <c r="AF5">
         <v>0.8</v>
       </c>
-      <c r="AD5">
-        <v>1</v>
-      </c>
-      <c r="AF5">
-        <v>1</v>
-      </c>
       <c r="AG5">
+        <v>1</v>
+      </c>
+      <c r="AI5">
+        <v>1</v>
+      </c>
+      <c r="AJ5">
         <v>5</v>
       </c>
-      <c r="AH5">
+      <c r="AK5">
         <v>6</v>
       </c>
-      <c r="AJ5">
+      <c r="AM5">
         <v>10</v>
       </c>
-      <c r="AK5">
+      <c r="AN5">
         <v>2</v>
       </c>
-      <c r="AL5">
+      <c r="AO5">
         <v>10</v>
       </c>
-      <c r="AM5">
+      <c r="AP5">
         <v>15</v>
       </c>
-      <c r="AN5">
+      <c r="AQ5">
         <v>21</v>
       </c>
-      <c r="AO5">
+      <c r="AR5">
         <v>2000</v>
       </c>
-      <c r="AP5">
+      <c r="AS5">
         <v>2000</v>
       </c>
-      <c r="AQ5">
-        <v>1</v>
-      </c>
-      <c r="AR5">
+      <c r="AT5">
+        <v>1</v>
+      </c>
+      <c r="AU5">
         <v>40</v>
       </c>
-      <c r="AS5">
+      <c r="AV5">
         <v>120</v>
       </c>
-      <c r="AT5">
+      <c r="AW5">
         <v>40</v>
       </c>
-      <c r="AU5">
+      <c r="AX5">
         <v>0.3</v>
       </c>
-      <c r="AV5">
+      <c r="AY5">
         <v>0.16</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="G6">
         <v>54</v>
       </c>
-      <c r="E6">
+      <c r="H6">
         <v>13700</v>
       </c>
-      <c r="F6">
+      <c r="I6">
         <v>2437.5</v>
       </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
         <v>0.15</v>
       </c>
-      <c r="I6">
+      <c r="L6">
         <v>0.9</v>
       </c>
-      <c r="J6">
+      <c r="M6">
         <v>7.4</v>
       </c>
-      <c r="K6">
+      <c r="N6">
         <v>0.9</v>
       </c>
-      <c r="M6" t="s">
-        <v>59</v>
-      </c>
-      <c r="N6" t="s">
+      <c r="P6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q6" t="s">
         <v>48</v>
       </c>
-      <c r="O6">
+      <c r="R6">
         <v>4</v>
       </c>
-      <c r="P6">
-        <v>1</v>
-      </c>
-      <c r="R6">
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="U6">
         <v>0.2</v>
       </c>
-      <c r="S6" s="1">
+      <c r="V6" s="1">
         <v>43521.791666666664</v>
       </c>
-      <c r="T6" s="1">
+      <c r="W6" s="1">
         <v>43524.291666666664</v>
       </c>
-      <c r="U6" t="s">
+      <c r="X6" t="s">
         <v>49</v>
       </c>
-      <c r="V6" t="s">
+      <c r="Y6" t="s">
         <v>50</v>
       </c>
-      <c r="X6" t="s">
+      <c r="AA6" t="s">
         <v>51</v>
       </c>
-      <c r="Y6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD6" t="s">
         <v>56</v>
       </c>
-      <c r="AB6">
+      <c r="AE6">
         <v>9</v>
       </c>
-      <c r="AC6">
+      <c r="AF6">
         <v>0.8</v>
       </c>
-      <c r="AD6">
+      <c r="AG6">
         <v>0</v>
       </c>
-      <c r="AF6">
-        <v>1</v>
-      </c>
-      <c r="AG6">
+      <c r="AI6">
+        <v>1</v>
+      </c>
+      <c r="AJ6">
         <v>5</v>
       </c>
-      <c r="AH6">
+      <c r="AK6">
         <v>6</v>
       </c>
-      <c r="AJ6">
+      <c r="AM6">
         <v>10</v>
       </c>
-      <c r="AK6">
+      <c r="AN6">
         <v>2</v>
       </c>
-      <c r="AL6">
+      <c r="AO6">
         <v>10</v>
       </c>
-      <c r="AM6">
+      <c r="AP6">
         <v>15</v>
       </c>
-      <c r="AN6">
+      <c r="AQ6">
         <v>21</v>
       </c>
-      <c r="AO6">
+      <c r="AR6">
         <v>2000</v>
       </c>
-      <c r="AP6">
+      <c r="AS6">
         <v>2000</v>
       </c>
-      <c r="AQ6">
-        <v>1</v>
-      </c>
-      <c r="AR6">
+      <c r="AT6">
+        <v>1</v>
+      </c>
+      <c r="AU6">
         <v>40</v>
       </c>
-      <c r="AS6">
+      <c r="AV6">
         <v>120</v>
       </c>
-      <c r="AT6">
+      <c r="AW6">
         <v>40</v>
       </c>
-      <c r="AU6">
+      <c r="AX6">
         <v>0.3</v>
       </c>
-      <c r="AV6">
+      <c r="AY6">
         <v>0.16</v>
       </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7">
+        <v>69</v>
+      </c>
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="G7">
         <v>54</v>
       </c>
-      <c r="E7">
+      <c r="H7">
         <v>13700</v>
       </c>
-      <c r="F7">
+      <c r="I7">
         <v>2437.5</v>
       </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
         <v>0.15</v>
       </c>
-      <c r="I7">
+      <c r="L7">
         <v>0.9</v>
       </c>
-      <c r="J7">
+      <c r="M7">
         <v>7.4</v>
       </c>
-      <c r="K7">
+      <c r="N7">
         <v>0.9</v>
       </c>
-      <c r="M7" t="s">
-        <v>59</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="P7" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q7" t="s">
         <v>48</v>
       </c>
-      <c r="O7">
+      <c r="R7">
         <v>4</v>
       </c>
-      <c r="P7">
-        <v>1</v>
-      </c>
-      <c r="R7">
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="U7">
         <v>0.2</v>
       </c>
-      <c r="S7" s="1">
+      <c r="V7" s="1">
         <v>43521.791666666664</v>
       </c>
-      <c r="T7" s="1">
+      <c r="W7" s="1">
         <v>43524.291666666664</v>
       </c>
-      <c r="U7" t="s">
+      <c r="X7" t="s">
         <v>49</v>
       </c>
-      <c r="V7" t="s">
+      <c r="Y7" t="s">
         <v>50</v>
       </c>
-      <c r="X7" t="s">
+      <c r="AA7" t="s">
         <v>51</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="AB7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE7">
+        <v>9</v>
+      </c>
+      <c r="AF7">
+        <v>0.8</v>
+      </c>
+      <c r="AG7">
+        <v>1</v>
+      </c>
+      <c r="AI7">
+        <v>1</v>
+      </c>
+      <c r="AJ7">
+        <v>5</v>
+      </c>
+      <c r="AK7">
+        <v>6</v>
+      </c>
+      <c r="AM7">
+        <v>10</v>
+      </c>
+      <c r="AN7">
+        <v>2</v>
+      </c>
+      <c r="AO7">
+        <v>10</v>
+      </c>
+      <c r="AP7">
+        <v>15</v>
+      </c>
+      <c r="AQ7">
+        <v>21</v>
+      </c>
+      <c r="AR7">
+        <v>2000</v>
+      </c>
+      <c r="AS7">
+        <v>2000</v>
+      </c>
+      <c r="AT7">
+        <v>1</v>
+      </c>
+      <c r="AU7">
+        <v>40</v>
+      </c>
+      <c r="AV7">
+        <v>120</v>
+      </c>
+      <c r="AW7">
+        <v>40</v>
+      </c>
+      <c r="AX7">
+        <v>0.3</v>
+      </c>
+      <c r="AY7">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>54</v>
+      </c>
+      <c r="H8">
+        <v>13700</v>
+      </c>
+      <c r="I8">
+        <v>2437.5</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>0.15</v>
+      </c>
+      <c r="L8">
+        <v>0.9</v>
+      </c>
+      <c r="M8">
+        <v>7.4</v>
+      </c>
+      <c r="N8">
+        <v>0.9</v>
+      </c>
+      <c r="P8" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>48</v>
+      </c>
+      <c r="R8">
+        <v>4</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>0.2</v>
+      </c>
+      <c r="V8" s="1">
+        <v>43521.791666666664</v>
+      </c>
+      <c r="W8" s="1">
+        <v>43524.291666666664</v>
+      </c>
+      <c r="X8" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB8" t="s">
         <v>55</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AD8" t="s">
         <v>56</v>
       </c>
-      <c r="AB7">
+      <c r="AE8">
         <v>9</v>
       </c>
-      <c r="AC7">
+      <c r="AF8">
         <v>0.8</v>
       </c>
-      <c r="AD7">
-        <v>1</v>
-      </c>
-      <c r="AF7">
-        <v>1</v>
-      </c>
-      <c r="AG7">
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
+        <v>1</v>
+      </c>
+      <c r="AJ8">
         <v>5</v>
       </c>
-      <c r="AH7">
+      <c r="AK8">
         <v>6</v>
       </c>
-      <c r="AJ7">
+      <c r="AM8">
         <v>10</v>
       </c>
-      <c r="AK7">
+      <c r="AN8">
         <v>2</v>
       </c>
-      <c r="AL7">
+      <c r="AO8">
         <v>10</v>
       </c>
-      <c r="AM7">
+      <c r="AP8">
         <v>15</v>
       </c>
-      <c r="AN7">
+      <c r="AQ8">
         <v>21</v>
       </c>
-      <c r="AO7">
+      <c r="AR8">
         <v>2000</v>
       </c>
-      <c r="AP7">
+      <c r="AS8">
         <v>2000</v>
       </c>
-      <c r="AQ7">
-        <v>1</v>
-      </c>
-      <c r="AR7">
+      <c r="AT8">
+        <v>1</v>
+      </c>
+      <c r="AU8">
         <v>40</v>
       </c>
-      <c r="AS7">
+      <c r="AV8">
         <v>120</v>
       </c>
-      <c r="AT7">
+      <c r="AW8">
         <v>40</v>
       </c>
-      <c r="AU7">
+      <c r="AX8">
         <v>0.3</v>
       </c>
-      <c r="AV7">
+      <c r="AY8">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>54</v>
+      </c>
+      <c r="H9">
+        <v>13700</v>
+      </c>
+      <c r="I9">
+        <v>2437.5</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>0.15</v>
+      </c>
+      <c r="L9">
+        <v>0.9</v>
+      </c>
+      <c r="M9">
+        <v>7.4</v>
+      </c>
+      <c r="N9">
+        <v>0.9</v>
+      </c>
+      <c r="P9" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>48</v>
+      </c>
+      <c r="R9">
+        <v>4</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="U9">
+        <v>0.2</v>
+      </c>
+      <c r="V9" s="1">
+        <v>43521.791666666664</v>
+      </c>
+      <c r="W9" s="1">
+        <v>43524.291666666664</v>
+      </c>
+      <c r="X9" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE9">
+        <v>9</v>
+      </c>
+      <c r="AF9">
+        <v>0.8</v>
+      </c>
+      <c r="AG9">
+        <v>1</v>
+      </c>
+      <c r="AI9">
+        <v>1</v>
+      </c>
+      <c r="AJ9">
+        <v>5</v>
+      </c>
+      <c r="AK9">
+        <v>6</v>
+      </c>
+      <c r="AM9">
+        <v>10</v>
+      </c>
+      <c r="AN9">
+        <v>2</v>
+      </c>
+      <c r="AO9">
+        <v>10</v>
+      </c>
+      <c r="AP9">
+        <v>15</v>
+      </c>
+      <c r="AQ9">
+        <v>21</v>
+      </c>
+      <c r="AR9">
+        <v>2000</v>
+      </c>
+      <c r="AS9">
+        <v>2000</v>
+      </c>
+      <c r="AT9">
+        <v>1</v>
+      </c>
+      <c r="AU9">
+        <v>40</v>
+      </c>
+      <c r="AV9">
+        <v>120</v>
+      </c>
+      <c r="AW9">
+        <v>40</v>
+      </c>
+      <c r="AX9">
+        <v>0.3</v>
+      </c>
+      <c r="AY9">
         <v>0.16</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A3:AV7">
+  <conditionalFormatting sqref="AC4:AY4 AC6:AY6 A3:B7 Q3:AY3 D3:O5 Q7:AY7 Q6:T6 D6:P7 Q5:AY5 Q4:T4 P2:P5">
+    <cfRule type="expression" dxfId="6" priority="10" stopIfTrue="1">
+      <formula>A2&lt;&gt;A1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W2:W9">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="lessThan">
+      <formula>V2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V2:W2">
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+      <formula>V2&lt;&gt;V1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V4:W4">
+    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+      <formula>V4&lt;&gt;V3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V6:W6">
+    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+      <formula>V6&lt;&gt;V5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC8:AY8 A8:B9 Q9:AY9 Q8:T8 D8:P9">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+      <formula>A8&lt;&gt;A7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V8:W8">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
-      <formula>A3&lt;&gt;A2</formula>
+      <formula>V8&lt;&gt;V7</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Reformatted PCS output file quickly
</commit_message>
<xml_diff>
--- a/Inputs/InputSchedule.xlsx
+++ b/Inputs/InputSchedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/ah17992_bristol_ac_uk/Documents/DP5/Shared/DP5_modelling/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="13_ncr:4000b_{DEB44F97-88D2-433A-B317-5E3E680ACB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69EBE43E-59F8-480A-B057-375AA2A6573F}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="13_ncr:4000b_{DEB44F97-88D2-433A-B317-5E3E680ACB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{591FA145-5550-486A-B65C-22F97F4BB062}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1167,7 +1167,7 @@
   <dimension ref="A1:AY9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="AT14" sqref="AT14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Still working after major carbon changes
</commit_message>
<xml_diff>
--- a/Inputs/InputSchedule.xlsx
+++ b/Inputs/InputSchedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/ah17992_bristol_ac_uk/Documents/DP5/Shared/DP5_modelling/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="121" documentId="13_ncr:4000b_{DEB44F97-88D2-433A-B317-5E3E680ACB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A097FA2D-D8D9-42E7-9C22-7D38F7D731F6}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="13_ncr:4000b_{DEB44F97-88D2-433A-B317-5E3E680ACB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64C45221-58EC-4031-B4B3-F2CB8157DE0E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="71">
   <si>
     <t>Case</t>
   </si>
@@ -236,7 +236,13 @@
     <t>CombinedCO2.csv</t>
   </si>
   <si>
-    <t>Battery Carbon</t>
+    <t>Battery Carbon per kWh</t>
+  </si>
+  <si>
+    <t>Battery Motivation</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
 </sst>
 </file>
@@ -1158,10 +1164,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BA9"/>
+  <dimension ref="A1:BB9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AW20" sqref="AW20"/>
+      <selection activeCell="AH5" sqref="AH5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1191,24 +1197,25 @@
     <col min="28" max="28" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="4" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="39" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="41" max="45" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="46" max="47" width="5" bestFit="1" customWidth="1"/>
-    <col min="48" max="49" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="4" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="4" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.28515625" customWidth="1"/>
+    <col min="32" max="32" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="4" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="40" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="42" max="46" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="48" width="5" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="4" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="4" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" s="5" customFormat="1" ht="122.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54" s="5" customFormat="1" ht="122.25" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>59</v>
       </c>
@@ -1299,77 +1306,80 @@
       <c r="AD1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AI1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AI1" s="7" t="s">
+      <c r="AJ1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="AL1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AM1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AN1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AP1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AP1" s="5" t="s">
+      <c r="AQ1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AQ1" s="5" t="s">
+      <c r="AR1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AR1" s="5" t="s">
+      <c r="AS1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AS1" s="5" t="s">
+      <c r="AT1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AT1" s="5" t="s">
+      <c r="AU1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AU1" s="5" t="s">
+      <c r="AV1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AV1" s="5" t="s">
+      <c r="AW1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AW1" s="5" t="s">
+      <c r="AX1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AX1" s="5" t="s">
+      <c r="AY1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AY1" s="5" t="s">
+      <c r="AZ1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AZ1" s="5" t="s">
+      <c r="BA1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="BA1" s="5" t="s">
+      <c r="BB1" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1410,7 +1420,7 @@
         <v>0.9</v>
       </c>
       <c r="Q2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="R2" t="s">
         <v>48</v>
@@ -1443,70 +1453,73 @@
         <v>51</v>
       </c>
       <c r="AD2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG2" t="s">
         <v>56</v>
       </c>
-      <c r="AG2">
+      <c r="AH2">
         <v>9</v>
       </c>
-      <c r="AH2">
+      <c r="AI2">
         <v>0.8</v>
       </c>
-      <c r="AI2">
+      <c r="AJ2">
         <v>0</v>
       </c>
-      <c r="AK2">
-        <v>1</v>
-      </c>
       <c r="AL2">
+        <v>1</v>
+      </c>
+      <c r="AM2">
         <v>5</v>
       </c>
-      <c r="AM2">
+      <c r="AN2">
         <v>6</v>
       </c>
-      <c r="AO2">
+      <c r="AP2">
         <v>10</v>
       </c>
-      <c r="AP2">
+      <c r="AQ2">
         <v>2</v>
       </c>
-      <c r="AQ2">
+      <c r="AR2">
         <v>10</v>
       </c>
-      <c r="AR2">
+      <c r="AS2">
         <v>15</v>
       </c>
-      <c r="AS2">
+      <c r="AT2">
         <v>21</v>
-      </c>
-      <c r="AT2">
-        <v>2000</v>
       </c>
       <c r="AU2">
         <v>2000</v>
       </c>
       <c r="AV2">
-        <v>1</v>
+        <v>2000</v>
       </c>
       <c r="AW2">
+        <v>1</v>
+      </c>
+      <c r="AX2">
         <v>40</v>
       </c>
-      <c r="AX2">
+      <c r="AY2">
         <v>120</v>
       </c>
-      <c r="AY2">
+      <c r="AZ2">
         <v>40</v>
       </c>
-      <c r="AZ2">
+      <c r="BA2">
         <v>0.3</v>
       </c>
-      <c r="BA2">
+      <c r="BB2">
         <v>0.16</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1582,68 +1595,71 @@
       <c r="AD3" t="s">
         <v>52</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AE3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG3" t="s">
         <v>56</v>
       </c>
-      <c r="AG3">
+      <c r="AH3">
         <v>9</v>
       </c>
-      <c r="AH3">
+      <c r="AI3">
         <v>0.8</v>
       </c>
-      <c r="AI3">
+      <c r="AJ3">
         <v>0</v>
       </c>
-      <c r="AK3">
-        <v>1</v>
-      </c>
       <c r="AL3">
+        <v>1</v>
+      </c>
+      <c r="AM3">
         <v>5</v>
       </c>
-      <c r="AM3">
+      <c r="AN3">
         <v>6</v>
       </c>
-      <c r="AO3">
+      <c r="AP3">
         <v>10</v>
       </c>
-      <c r="AP3">
+      <c r="AQ3">
         <v>2</v>
       </c>
-      <c r="AQ3">
+      <c r="AR3">
         <v>10</v>
       </c>
-      <c r="AR3">
+      <c r="AS3">
         <v>15</v>
       </c>
-      <c r="AS3">
+      <c r="AT3">
         <v>21</v>
-      </c>
-      <c r="AT3">
-        <v>2000</v>
       </c>
       <c r="AU3">
         <v>2000</v>
       </c>
       <c r="AV3">
-        <v>1</v>
+        <v>2000</v>
       </c>
       <c r="AW3">
+        <v>1</v>
+      </c>
+      <c r="AX3">
         <v>40</v>
       </c>
-      <c r="AX3">
+      <c r="AY3">
         <v>120</v>
       </c>
-      <c r="AY3">
+      <c r="AZ3">
         <v>40</v>
       </c>
-      <c r="AZ3">
+      <c r="BA3">
         <v>0.3</v>
       </c>
-      <c r="BA3">
+      <c r="BB3">
         <v>0.16</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1719,68 +1735,71 @@
       <c r="AD4" t="s">
         <v>55</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AE4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG4" t="s">
         <v>53</v>
       </c>
-      <c r="AG4">
+      <c r="AH4">
         <v>9</v>
       </c>
-      <c r="AH4">
+      <c r="AI4">
         <v>0.8</v>
       </c>
-      <c r="AI4">
+      <c r="AJ4">
         <v>0</v>
       </c>
-      <c r="AK4">
-        <v>1</v>
-      </c>
       <c r="AL4">
+        <v>1</v>
+      </c>
+      <c r="AM4">
         <v>5</v>
       </c>
-      <c r="AM4">
+      <c r="AN4">
         <v>6</v>
       </c>
-      <c r="AO4">
+      <c r="AP4">
         <v>10</v>
       </c>
-      <c r="AP4">
+      <c r="AQ4">
         <v>2</v>
       </c>
-      <c r="AQ4">
+      <c r="AR4">
         <v>10</v>
       </c>
-      <c r="AR4">
+      <c r="AS4">
         <v>15</v>
       </c>
-      <c r="AS4">
+      <c r="AT4">
         <v>21</v>
-      </c>
-      <c r="AT4">
-        <v>2000</v>
       </c>
       <c r="AU4">
         <v>2000</v>
       </c>
       <c r="AV4">
-        <v>1</v>
+        <v>2000</v>
       </c>
       <c r="AW4">
+        <v>1</v>
+      </c>
+      <c r="AX4">
         <v>40</v>
       </c>
-      <c r="AX4">
+      <c r="AY4">
         <v>120</v>
       </c>
-      <c r="AY4">
+      <c r="AZ4">
         <v>40</v>
       </c>
-      <c r="AZ4">
+      <c r="BA4">
         <v>0.3</v>
       </c>
-      <c r="BA4">
+      <c r="BB4">
         <v>0.16</v>
       </c>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1856,68 +1875,71 @@
       <c r="AD5" t="s">
         <v>52</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AE5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG5" t="s">
         <v>53</v>
       </c>
-      <c r="AG5">
+      <c r="AH5">
         <v>9</v>
       </c>
-      <c r="AH5">
+      <c r="AI5">
         <v>0.8</v>
       </c>
-      <c r="AI5">
+      <c r="AJ5">
         <v>0</v>
       </c>
-      <c r="AK5">
-        <v>1</v>
-      </c>
       <c r="AL5">
+        <v>1</v>
+      </c>
+      <c r="AM5">
         <v>5</v>
       </c>
-      <c r="AM5">
+      <c r="AN5">
         <v>6</v>
       </c>
-      <c r="AO5">
+      <c r="AP5">
         <v>10</v>
       </c>
-      <c r="AP5">
+      <c r="AQ5">
         <v>2</v>
       </c>
-      <c r="AQ5">
+      <c r="AR5">
         <v>10</v>
       </c>
-      <c r="AR5">
+      <c r="AS5">
         <v>15</v>
       </c>
-      <c r="AS5">
+      <c r="AT5">
         <v>21</v>
-      </c>
-      <c r="AT5">
-        <v>2000</v>
       </c>
       <c r="AU5">
         <v>2000</v>
       </c>
       <c r="AV5">
-        <v>1</v>
+        <v>2000</v>
       </c>
       <c r="AW5">
+        <v>1</v>
+      </c>
+      <c r="AX5">
         <v>40</v>
       </c>
-      <c r="AX5">
+      <c r="AY5">
         <v>120</v>
       </c>
-      <c r="AY5">
+      <c r="AZ5">
         <v>40</v>
       </c>
-      <c r="AZ5">
+      <c r="BA5">
         <v>0.3</v>
       </c>
-      <c r="BA5">
+      <c r="BB5">
         <v>0.16</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1993,68 +2015,71 @@
       <c r="AD6" t="s">
         <v>55</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AE6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG6" t="s">
         <v>56</v>
       </c>
-      <c r="AG6">
+      <c r="AH6">
         <v>9</v>
       </c>
-      <c r="AH6">
+      <c r="AI6">
         <v>0.8</v>
       </c>
-      <c r="AI6">
+      <c r="AJ6">
         <v>0</v>
       </c>
-      <c r="AK6">
-        <v>1</v>
-      </c>
       <c r="AL6">
+        <v>1</v>
+      </c>
+      <c r="AM6">
         <v>5</v>
       </c>
-      <c r="AM6">
+      <c r="AN6">
         <v>6</v>
       </c>
-      <c r="AO6">
+      <c r="AP6">
         <v>10</v>
       </c>
-      <c r="AP6">
+      <c r="AQ6">
         <v>2</v>
       </c>
-      <c r="AQ6">
+      <c r="AR6">
         <v>10</v>
       </c>
-      <c r="AR6">
+      <c r="AS6">
         <v>15</v>
       </c>
-      <c r="AS6">
+      <c r="AT6">
         <v>21</v>
-      </c>
-      <c r="AT6">
-        <v>2000</v>
       </c>
       <c r="AU6">
         <v>2000</v>
       </c>
       <c r="AV6">
-        <v>1</v>
+        <v>2000</v>
       </c>
       <c r="AW6">
+        <v>1</v>
+      </c>
+      <c r="AX6">
         <v>40</v>
       </c>
-      <c r="AX6">
+      <c r="AY6">
         <v>120</v>
       </c>
-      <c r="AY6">
+      <c r="AZ6">
         <v>40</v>
       </c>
-      <c r="AZ6">
+      <c r="BA6">
         <v>0.3</v>
       </c>
-      <c r="BA6">
+      <c r="BB6">
         <v>0.16</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -2130,68 +2155,71 @@
       <c r="AD7" t="s">
         <v>52</v>
       </c>
-      <c r="AF7" t="s">
+      <c r="AE7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG7" t="s">
         <v>56</v>
       </c>
-      <c r="AG7">
+      <c r="AH7">
         <v>9</v>
       </c>
-      <c r="AH7">
+      <c r="AI7">
         <v>0.8</v>
       </c>
-      <c r="AI7">
+      <c r="AJ7">
         <v>0</v>
       </c>
-      <c r="AK7">
-        <v>1</v>
-      </c>
       <c r="AL7">
+        <v>1</v>
+      </c>
+      <c r="AM7">
         <v>5</v>
       </c>
-      <c r="AM7">
+      <c r="AN7">
         <v>6</v>
       </c>
-      <c r="AO7">
+      <c r="AP7">
         <v>10</v>
       </c>
-      <c r="AP7">
+      <c r="AQ7">
         <v>2</v>
       </c>
-      <c r="AQ7">
+      <c r="AR7">
         <v>10</v>
       </c>
-      <c r="AR7">
+      <c r="AS7">
         <v>15</v>
       </c>
-      <c r="AS7">
+      <c r="AT7">
         <v>21</v>
-      </c>
-      <c r="AT7">
-        <v>2000</v>
       </c>
       <c r="AU7">
         <v>2000</v>
       </c>
       <c r="AV7">
-        <v>1</v>
+        <v>2000</v>
       </c>
       <c r="AW7">
+        <v>1</v>
+      </c>
+      <c r="AX7">
         <v>40</v>
       </c>
-      <c r="AX7">
+      <c r="AY7">
         <v>120</v>
       </c>
-      <c r="AY7">
+      <c r="AZ7">
         <v>40</v>
       </c>
-      <c r="AZ7">
+      <c r="BA7">
         <v>0.3</v>
       </c>
-      <c r="BA7">
+      <c r="BB7">
         <v>0.16</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -2267,68 +2295,71 @@
       <c r="AD8" t="s">
         <v>55</v>
       </c>
-      <c r="AF8" t="s">
+      <c r="AE8" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG8" t="s">
         <v>56</v>
       </c>
-      <c r="AG8">
+      <c r="AH8">
         <v>9</v>
       </c>
-      <c r="AH8">
+      <c r="AI8">
         <v>0.8</v>
       </c>
-      <c r="AI8">
+      <c r="AJ8">
         <v>0</v>
       </c>
-      <c r="AK8">
-        <v>1</v>
-      </c>
       <c r="AL8">
+        <v>1</v>
+      </c>
+      <c r="AM8">
         <v>5</v>
       </c>
-      <c r="AM8">
+      <c r="AN8">
         <v>6</v>
       </c>
-      <c r="AO8">
+      <c r="AP8">
         <v>10</v>
       </c>
-      <c r="AP8">
+      <c r="AQ8">
         <v>2</v>
       </c>
-      <c r="AQ8">
+      <c r="AR8">
         <v>10</v>
       </c>
-      <c r="AR8">
+      <c r="AS8">
         <v>15</v>
       </c>
-      <c r="AS8">
+      <c r="AT8">
         <v>21</v>
-      </c>
-      <c r="AT8">
-        <v>2000</v>
       </c>
       <c r="AU8">
         <v>2000</v>
       </c>
       <c r="AV8">
-        <v>1</v>
+        <v>2000</v>
       </c>
       <c r="AW8">
+        <v>1</v>
+      </c>
+      <c r="AX8">
         <v>40</v>
       </c>
-      <c r="AX8">
+      <c r="AY8">
         <v>120</v>
       </c>
-      <c r="AY8">
+      <c r="AZ8">
         <v>40</v>
       </c>
-      <c r="AZ8">
+      <c r="BA8">
         <v>0.3</v>
       </c>
-      <c r="BA8">
+      <c r="BB8">
         <v>0.16</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -2404,70 +2435,73 @@
       <c r="AD9" t="s">
         <v>52</v>
       </c>
-      <c r="AF9" t="s">
+      <c r="AE9" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG9" t="s">
         <v>56</v>
       </c>
-      <c r="AG9">
+      <c r="AH9">
         <v>9</v>
       </c>
-      <c r="AH9">
+      <c r="AI9">
         <v>0.8</v>
       </c>
-      <c r="AI9">
+      <c r="AJ9">
         <v>0</v>
       </c>
-      <c r="AK9">
-        <v>1</v>
-      </c>
       <c r="AL9">
+        <v>1</v>
+      </c>
+      <c r="AM9">
         <v>5</v>
       </c>
-      <c r="AM9">
+      <c r="AN9">
         <v>6</v>
       </c>
-      <c r="AO9">
+      <c r="AP9">
         <v>10</v>
       </c>
-      <c r="AP9">
+      <c r="AQ9">
         <v>2</v>
       </c>
-      <c r="AQ9">
+      <c r="AR9">
         <v>10</v>
       </c>
-      <c r="AR9">
+      <c r="AS9">
         <v>15</v>
       </c>
-      <c r="AS9">
+      <c r="AT9">
         <v>21</v>
-      </c>
-      <c r="AT9">
-        <v>2000</v>
       </c>
       <c r="AU9">
         <v>2000</v>
       </c>
       <c r="AV9">
-        <v>1</v>
+        <v>2000</v>
       </c>
       <c r="AW9">
+        <v>1</v>
+      </c>
+      <c r="AX9">
         <v>40</v>
       </c>
-      <c r="AX9">
+      <c r="AY9">
         <v>120</v>
       </c>
-      <c r="AY9">
+      <c r="AZ9">
         <v>40</v>
       </c>
-      <c r="AZ9">
+      <c r="BA9">
         <v>0.3</v>
       </c>
-      <c r="BA9">
+      <c r="BB9">
         <v>0.16</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="AE4:BA4 AE6:BA6 A3:B7 R3:R7 Q2:Q5 T4:V4 T5:BA5 T6:V6 T7:BA7 T3:BA3 I3:P5 D3:G7 I6:Q7">
+  <conditionalFormatting sqref="A3:B7 R3:R7 T4:V4 T5:AD5 T6:V6 T7:AD7 T3:AD3 I3:P5 D3:G7 I6:Q7 Q2:Q5 AF3:BB7">
     <cfRule type="expression" dxfId="6" priority="10" stopIfTrue="1">
       <formula>A2&lt;&gt;A1</formula>
     </cfRule>
@@ -2492,7 +2526,7 @@
       <formula>X6&lt;&gt;X5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE8:BA8 A8:B9 T8:V8 T9:BA9 D8:G9 I8:R9">
+  <conditionalFormatting sqref="A8:B9 T8:V8 T9:AD9 D8:G9 I8:R9 AF8:BB9">
     <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>A8&lt;&gt;A7</formula>
     </cfRule>

</xml_diff>

<commit_message>
Somehow fully working. Can now motivate by carbon reduction and return carbon emitted and cost separately
</commit_message>
<xml_diff>
--- a/Inputs/InputSchedule.xlsx
+++ b/Inputs/InputSchedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/ah17992_bristol_ac_uk/Documents/DP5/Shared/DP5_modelling/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="138" documentId="13_ncr:4000b_{DEB44F97-88D2-433A-B317-5E3E680ACB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64C45221-58EC-4031-B4B3-F2CB8157DE0E}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="13_ncr:4000b_{DEB44F97-88D2-433A-B317-5E3E680ACB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEAC2463-B634-4C5A-88FC-3D1919C76820}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="72">
   <si>
     <t>Case</t>
   </si>
@@ -194,55 +194,58 @@
     <t>Electric</t>
   </si>
   <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>Electric Heater</t>
+  </si>
+  <si>
+    <t>Fixed22Tariff.csv</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Current Household of 4</t>
+  </si>
+  <si>
+    <t>Costs</t>
+  </si>
+  <si>
+    <t>Cost of Change</t>
+  </si>
+  <si>
+    <t>Agile Tariff</t>
+  </si>
+  <si>
+    <t>Carbon Intensity</t>
+  </si>
+  <si>
+    <t>CombinedCO2.csv</t>
+  </si>
+  <si>
+    <t>Battery Carbon per kWh</t>
+  </si>
+  <si>
+    <t>Battery Motivation</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Carbon</t>
+  </si>
+  <si>
+    <t>Carbon Motivated</t>
+  </si>
+  <si>
     <t>Datum</t>
-  </si>
-  <si>
-    <t>Home</t>
-  </si>
-  <si>
-    <t>Gas</t>
-  </si>
-  <si>
-    <t>Electric Heater</t>
-  </si>
-  <si>
-    <t>Fixed22Tariff.csv</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Current Household of 4</t>
-  </si>
-  <si>
-    <t>Costs</t>
-  </si>
-  <si>
-    <t>Cost of Change</t>
-  </si>
-  <si>
-    <t>Agile Tariff</t>
-  </si>
-  <si>
-    <t>Fourth</t>
-  </si>
-  <si>
-    <t>Carbon Intensity</t>
-  </si>
-  <si>
-    <t>CombinedCO2.csv</t>
-  </si>
-  <si>
-    <t>Battery Carbon per kWh</t>
-  </si>
-  <si>
-    <t>Battery Motivation</t>
-  </si>
-  <si>
-    <t>Price</t>
   </si>
 </sst>
 </file>
@@ -1167,7 +1170,7 @@
   <dimension ref="A1:BB9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AH5" sqref="AH5"/>
+      <selection activeCell="AI3" sqref="AI3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1217,19 +1220,19 @@
   <sheetData>
     <row r="1" spans="1:54" s="5" customFormat="1" ht="122.25" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>1</v>
@@ -1238,7 +1241,7 @@
         <v>2</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>3</v>
@@ -1271,7 +1274,7 @@
         <v>12</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="T1" s="5" t="s">
         <v>13</v>
@@ -1307,7 +1310,7 @@
         <v>23</v>
       </c>
       <c r="AE1" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AF1" s="3" t="s">
         <v>24</v>
@@ -1384,10 +1387,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1426,7 +1429,7 @@
         <v>48</v>
       </c>
       <c r="S2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T2">
         <v>4</v>
@@ -1456,10 +1459,10 @@
         <v>52</v>
       </c>
       <c r="AE2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AG2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AH2">
         <v>9</v>
@@ -1468,7 +1471,7 @@
         <v>0.8</v>
       </c>
       <c r="AJ2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL2">
         <v>1</v>
@@ -1524,10 +1527,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1560,13 +1563,13 @@
         <v>0.9</v>
       </c>
       <c r="Q3" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="R3" t="s">
         <v>48</v>
       </c>
       <c r="S3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T3">
         <v>4</v>
@@ -1596,10 +1599,10 @@
         <v>52</v>
       </c>
       <c r="AE3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AG3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AH3">
         <v>9</v>
@@ -1608,7 +1611,7 @@
         <v>0.8</v>
       </c>
       <c r="AJ3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL3">
         <v>1</v>
@@ -1664,13 +1667,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>54</v>
@@ -1700,13 +1703,13 @@
         <v>0.9</v>
       </c>
       <c r="Q4" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="R4" t="s">
         <v>48</v>
       </c>
       <c r="S4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T4">
         <v>4</v>
@@ -1733,13 +1736,13 @@
         <v>51</v>
       </c>
       <c r="AD4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG4" t="s">
         <v>55</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>53</v>
       </c>
       <c r="AH4">
         <v>9</v>
@@ -1748,7 +1751,7 @@
         <v>0.8</v>
       </c>
       <c r="AJ4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL4">
         <v>1</v>
@@ -1804,13 +1807,13 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>54</v>
@@ -1840,13 +1843,13 @@
         <v>0.9</v>
       </c>
       <c r="Q5" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="R5" t="s">
         <v>48</v>
       </c>
       <c r="S5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T5">
         <v>4</v>
@@ -1876,10 +1879,10 @@
         <v>52</v>
       </c>
       <c r="AE5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AG5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AH5">
         <v>9</v>
@@ -1888,7 +1891,7 @@
         <v>0.8</v>
       </c>
       <c r="AJ5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL5">
         <v>1</v>
@@ -1944,13 +1947,13 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="G6">
         <v>54</v>
@@ -1980,13 +1983,13 @@
         <v>0.9</v>
       </c>
       <c r="Q6" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="R6" t="s">
         <v>48</v>
       </c>
       <c r="S6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T6">
         <v>4</v>
@@ -2013,13 +2016,13 @@
         <v>51</v>
       </c>
       <c r="AD6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AE6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AG6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="AH6">
         <v>9</v>
@@ -2084,13 +2087,13 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="G7">
         <v>54</v>
@@ -2120,13 +2123,13 @@
         <v>0.9</v>
       </c>
       <c r="Q7" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="R7" t="s">
         <v>48</v>
       </c>
       <c r="S7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T7">
         <v>4</v>
@@ -2156,10 +2159,10 @@
         <v>52</v>
       </c>
       <c r="AE7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AG7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="AH7">
         <v>9</v>
@@ -2221,13 +2224,13 @@
     </row>
     <row r="8" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -2266,7 +2269,7 @@
         <v>48</v>
       </c>
       <c r="S8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T8">
         <v>4</v>
@@ -2293,13 +2296,13 @@
         <v>51</v>
       </c>
       <c r="AD8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG8" t="s">
         <v>55</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>70</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>56</v>
       </c>
       <c r="AH8">
         <v>9</v>
@@ -2361,13 +2364,13 @@
     </row>
     <row r="9" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -2406,7 +2409,7 @@
         <v>48</v>
       </c>
       <c r="S9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T9">
         <v>4</v>
@@ -2436,10 +2439,10 @@
         <v>52</v>
       </c>
       <c r="AE9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AG9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AH9">
         <v>9</v>
@@ -2501,39 +2504,39 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A3:B7 R3:R7 T4:V4 T5:AD5 T6:V6 T7:AD7 T3:AD3 I3:P5 D3:G7 I6:Q7 Q2:Q5 AF3:BB7">
-    <cfRule type="expression" dxfId="6" priority="10" stopIfTrue="1">
+  <conditionalFormatting sqref="T7:AD7 T8:V8 T9:AD9 A7:B9 D7:G9 AF7:BB9 I7:R9 Q2:Q5">
+    <cfRule type="expression" dxfId="6" priority="12" stopIfTrue="1">
       <formula>A2&lt;&gt;A1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y9">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="lessThan">
       <formula>X2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:Y2">
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="7" stopIfTrue="1">
       <formula>X2&lt;&gt;X1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X4:Y4">
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
-      <formula>X4&lt;&gt;X3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X6:Y6">
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
-      <formula>X6&lt;&gt;X5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8:B9 T8:V8 T9:AD9 D8:G9 I8:R9 AF8:BB9">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
-      <formula>A8&lt;&gt;A7</formula>
+  <conditionalFormatting sqref="X6:Y6 A6:B6 D6:G6 AF6:BB6 I6:R6 T6:V6">
+    <cfRule type="expression" dxfId="3" priority="6" stopIfTrue="1">
+      <formula>A6&lt;&gt;A3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X8:Y8">
+    <cfRule type="expression" dxfId="2" priority="5" stopIfTrue="1">
+      <formula>X8&lt;&gt;X7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X3:Y3 X5:Y5">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+      <formula>X3&lt;&gt;X2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X4:Y4">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
-      <formula>X8&lt;&gt;X7</formula>
+      <formula>X4&lt;&gt;X3</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Uses API to recalculate departure (plu out) time
</commit_message>
<xml_diff>
--- a/Inputs/InputSchedule.xlsx
+++ b/Inputs/InputSchedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/ah17992_bristol_ac_uk/Documents/DP5/Shared/DP5_modelling/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="254" documentId="13_ncr:4000b_{DEB44F97-88D2-433A-B317-5E3E680ACB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{131B2BC4-14AA-45CE-8C88-86670E437039}"/>
+  <xr:revisionPtr revIDLastSave="260" documentId="13_ncr:4000b_{DEB44F97-88D2-433A-B317-5E3E680ACB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{803E5058-B4C9-4ECC-B71F-4B692983E045}"/>
   <bookViews>
-    <workbookView xWindow="-330" yWindow="-450" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="510" yWindow="1485" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InputSchedule" sheetId="1" r:id="rId1"/>
@@ -852,7 +852,34 @@
     <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1225,7 +1252,7 @@
   <dimension ref="A1:BR15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Z27" sqref="Z27"/>
+      <selection activeCell="AL7" sqref="AL7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,7 +1279,8 @@
     <col min="24" max="25" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="31" width="3.7109375" customWidth="1"/>
+    <col min="28" max="30" width="3.7109375" customWidth="1"/>
+    <col min="31" max="31" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="3.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="6.28515625" bestFit="1" customWidth="1"/>
@@ -1558,6 +1586,9 @@
       <c r="AA2" t="s">
         <v>47</v>
       </c>
+      <c r="AE2" s="1">
+        <v>44255.291666666664</v>
+      </c>
       <c r="AG2" t="s">
         <v>48</v>
       </c>
@@ -1700,6 +1731,9 @@
       </c>
       <c r="AA3" t="s">
         <v>47</v>
+      </c>
+      <c r="AE3" s="1">
+        <v>43522.291666666664</v>
       </c>
       <c r="AG3" t="s">
         <v>48</v>
@@ -3456,44 +3490,59 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A3:XFD6 A8:A11 C8:AH11 A13:XFD15 AJ8:XFD11">
-    <cfRule type="expression" dxfId="7" priority="14" stopIfTrue="1">
+  <conditionalFormatting sqref="A8:A11 C8:AH11 A13:XFD15 AJ8:XFD11 A3:XFD6">
+    <cfRule type="expression" dxfId="10" priority="17" stopIfTrue="1">
       <formula>A3&lt;&gt;A2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y15">
-    <cfRule type="cellIs" dxfId="6" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="14" operator="lessThan">
       <formula>X2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:Y2">
-    <cfRule type="expression" dxfId="5" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="12" stopIfTrue="1">
       <formula>X2&lt;&gt;X1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X12:Y12 A12:B12 D12:G12 AJ12:BF12 I12:R12 T12:V12">
-    <cfRule type="expression" dxfId="4" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
       <formula>A12&lt;&gt;A3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X14:Y14">
-    <cfRule type="expression" dxfId="3" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="10" stopIfTrue="1">
       <formula>X14&lt;&gt;X13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X7:Y7">
-    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
       <formula>X7&lt;&gt;X6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:B11">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
       <formula>B7&lt;&gt;B1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:XFD12">
-    <cfRule type="expression" dxfId="0" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="20" stopIfTrue="1">
       <formula>A12&lt;&gt;#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE2">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+      <formula>AD2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE2">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+      <formula>AE2&lt;&gt;AE1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE3">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>AD3</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
debugging and reserve charge toggle added
</commit_message>
<xml_diff>
--- a/Inputs/InputSchedule.xlsx
+++ b/Inputs/InputSchedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yazzadsukhia/Desktop/DP5_new_mod/DP5_modelling/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D24411-AFB7-8440-AE8D-59E0E0CC4DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57505528-C0AC-AF43-B518-BDF5D0845882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14260" yWindow="500" windowWidth="21060" windowHeight="18640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8520" yWindow="500" windowWidth="26800" windowHeight="18640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InputSchedule" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="85">
   <si>
     <t>Case</t>
   </si>
@@ -81,12 +81,6 @@
     <t>Connection Properties</t>
   </si>
   <si>
-    <t>Reserve Charge Duration</t>
-  </si>
-  <si>
-    <t>Journey Charge Duration</t>
-  </si>
-  <si>
     <t>Simulation Properties</t>
   </si>
   <si>
@@ -171,12 +165,6 @@
     <t>AgileExport.csv</t>
   </si>
   <si>
-    <t>0.5 h</t>
-  </si>
-  <si>
-    <t>2 h</t>
-  </si>
-  <si>
     <t>15 min</t>
   </si>
   <si>
@@ -261,9 +249,6 @@
     <t>Destination Arrival Time</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Bristol, UK, BS8 2AB</t>
   </si>
   <si>
@@ -292,6 +277,15 @@
   </si>
   <si>
     <t>Cooling</t>
+  </si>
+  <si>
+    <t>London, UK, HA5 5SG</t>
+  </si>
+  <si>
+    <t>Electric</t>
+  </si>
+  <si>
+    <t>Carbon</t>
   </si>
 </sst>
 </file>
@@ -795,7 +789,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -815,18 +809,9 @@
       <alignment textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1242,10 +1227,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BT3"/>
+  <dimension ref="A1:BR3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1270,57 +1255,56 @@
     <col min="22" max="22" width="3.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="4" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="20.33203125" customWidth="1"/>
-    <col min="32" max="32" width="3.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="6.33203125" customWidth="1"/>
-    <col min="36" max="36" width="3.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.33203125" customWidth="1"/>
+    <col min="30" max="30" width="3.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.33203125" customWidth="1"/>
+    <col min="34" max="34" width="3.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="4" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="3.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="42" max="44" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="3.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="46" max="50" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="51" max="52" width="5" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="3.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="40" max="42" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="3.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="44" max="48" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="5" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="4" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="3.6640625" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="4" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="4" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="3.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="63" max="67" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="3.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="61" max="65" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="3.6640625" bestFit="1" customWidth="1"/>
     <col min="69" max="69" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="3.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:72" s="5" customFormat="1" ht="121">
+    <row r="1" spans="1:70" s="5" customFormat="1" ht="118">
       <c r="A1" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>1</v>
@@ -1329,7 +1313,7 @@
         <v>2</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>3</v>
@@ -1362,7 +1346,7 @@
         <v>12</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="T1" s="5" t="s">
         <v>13</v>
@@ -1374,72 +1358,72 @@
         <v>15</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="Y1" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z1" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AB1" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC1" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD1" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE1" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AF1" s="5" t="s">
         <v>18</v>
       </c>
       <c r="AG1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AI1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="AI1" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>21</v>
       </c>
       <c r="AK1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AL1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AM1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AN1" s="7" t="s">
+      <c r="AN1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AO1" s="5" t="s">
         <v>26</v>
       </c>
       <c r="AP1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AQ1" s="5" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>28</v>
       </c>
       <c r="AR1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AS1" s="5" t="s">
         <v>30</v>
       </c>
       <c r="AT1" s="5" t="s">
@@ -1475,64 +1459,58 @@
       <c r="BD1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="BE1" s="5" t="s">
-        <v>42</v>
+      <c r="BE1" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="BF1" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="BG1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="BG1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="BH1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="BI1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="BJ1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="BK1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="BL1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="BM1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="BN1" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="BO1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="BH1" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="BI1" s="5" t="s">
+      <c r="BP1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="BJ1" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="BK1" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="BL1" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="BM1" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="BN1" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="BO1" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="BP1" s="5" t="s">
-        <v>84</v>
-      </c>
       <c r="BQ1" s="5" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="BR1" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="BS1" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="BT1" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:72">
+    <row r="2" spans="1:70">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1565,13 +1543,13 @@
         <v>0.9</v>
       </c>
       <c r="Q2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="S2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="T2">
         <v>4</v>
@@ -1588,101 +1566,101 @@
       <c r="Y2" s="1">
         <v>44255.291666666664</v>
       </c>
-      <c r="Z2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA2" t="s">
+      <c r="Z2" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB2" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>44255.305555555555</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI2" t="s">
         <v>47</v>
       </c>
-      <c r="AB2" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="AC2" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="AD2" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="AE2" s="1">
-        <v>43522.305555555555</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>51</v>
+      <c r="AJ2">
+        <v>9</v>
+      </c>
+      <c r="AK2">
+        <v>0.8</v>
       </c>
       <c r="AL2">
-        <v>9</v>
-      </c>
-      <c r="AM2">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="AN2">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>5</v>
       </c>
       <c r="AP2">
-        <v>1</v>
-      </c>
-      <c r="AQ2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AR2">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="AS2">
+        <v>2</v>
       </c>
       <c r="AT2">
         <v>10</v>
       </c>
       <c r="AU2">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="AV2">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="AW2">
-        <v>15</v>
+        <v>2000</v>
       </c>
       <c r="AX2">
-        <v>21</v>
+        <v>2000</v>
       </c>
       <c r="AY2">
-        <v>2000</v>
+        <v>1</v>
       </c>
       <c r="AZ2">
-        <v>2000</v>
+        <v>40</v>
       </c>
       <c r="BA2">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="BB2">
         <v>40</v>
       </c>
       <c r="BC2">
-        <v>120</v>
+        <v>0.3</v>
       </c>
       <c r="BD2">
-        <v>40</v>
-      </c>
-      <c r="BE2">
-        <v>0.3</v>
+        <v>0.16</v>
       </c>
       <c r="BF2">
-        <v>0.16</v>
+        <v>1</v>
+      </c>
+      <c r="BG2">
+        <v>355</v>
       </c>
       <c r="BH2">
-        <v>1</v>
+        <v>1684</v>
       </c>
       <c r="BI2">
-        <v>355</v>
+        <v>1</v>
       </c>
       <c r="BJ2">
-        <v>1684</v>
+        <v>1</v>
       </c>
       <c r="BK2">
         <v>1</v>
@@ -1693,37 +1671,31 @@
       <c r="BM2">
         <v>1</v>
       </c>
-      <c r="BN2">
-        <v>1</v>
+      <c r="BN2" s="8">
+        <v>46.8</v>
       </c>
       <c r="BO2">
-        <v>1</v>
-      </c>
-      <c r="BP2" s="8">
-        <v>46.8</v>
+        <v>143</v>
+      </c>
+      <c r="BP2">
+        <v>23</v>
       </c>
       <c r="BQ2">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="BR2">
-        <v>23</v>
-      </c>
-      <c r="BS2">
-        <v>150</v>
-      </c>
-      <c r="BT2">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:72">
+    <row r="3" spans="1:70">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1756,13 +1728,13 @@
         <v>0.9</v>
       </c>
       <c r="Q3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="S3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="T3">
         <v>4</v>
@@ -1779,101 +1751,101 @@
       <c r="Y3" s="1">
         <v>43522.291666666664</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="Z3" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA3" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB3" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>43522.305555555555</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF3" t="s">
         <v>46</v>
       </c>
-      <c r="AA3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB3" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC3" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="AD3" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="AE3" s="1">
-        <v>43522.305555555555</v>
-      </c>
       <c r="AG3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>49</v>
+        <v>84</v>
       </c>
       <c r="AI3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>51</v>
+        <v>83</v>
+      </c>
+      <c r="AJ3">
+        <v>9</v>
+      </c>
+      <c r="AK3">
+        <v>0.8</v>
       </c>
       <c r="AL3">
-        <v>9</v>
-      </c>
-      <c r="AM3">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="AN3">
         <v>0</v>
       </c>
+      <c r="AO3">
+        <v>5</v>
+      </c>
       <c r="AP3">
-        <v>1</v>
-      </c>
-      <c r="AQ3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AR3">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="AS3">
+        <v>2</v>
       </c>
       <c r="AT3">
         <v>10</v>
       </c>
       <c r="AU3">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="AV3">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="AW3">
-        <v>15</v>
+        <v>2000</v>
       </c>
       <c r="AX3">
-        <v>21</v>
+        <v>2000</v>
       </c>
       <c r="AY3">
-        <v>2000</v>
+        <v>1</v>
       </c>
       <c r="AZ3">
-        <v>2000</v>
+        <v>40</v>
       </c>
       <c r="BA3">
-        <v>1</v>
+        <v>120</v>
       </c>
       <c r="BB3">
         <v>40</v>
       </c>
       <c r="BC3">
-        <v>120</v>
+        <v>0.3</v>
       </c>
       <c r="BD3">
-        <v>40</v>
-      </c>
-      <c r="BE3">
-        <v>0.3</v>
+        <v>0.16</v>
       </c>
       <c r="BF3">
-        <v>0.16</v>
+        <v>1</v>
+      </c>
+      <c r="BG3">
+        <v>355</v>
       </c>
       <c r="BH3">
-        <v>1</v>
+        <v>1684</v>
       </c>
       <c r="BI3">
-        <v>355</v>
+        <v>1</v>
       </c>
       <c r="BJ3">
-        <v>1684</v>
+        <v>1</v>
       </c>
       <c r="BK3">
         <v>1</v>
@@ -1884,63 +1856,57 @@
       <c r="BM3">
         <v>1</v>
       </c>
-      <c r="BN3">
-        <v>1</v>
+      <c r="BN3" s="8">
+        <v>46.8</v>
       </c>
       <c r="BO3">
-        <v>1</v>
-      </c>
-      <c r="BP3" s="8">
-        <v>46.8</v>
+        <v>143</v>
+      </c>
+      <c r="BP3">
+        <v>23</v>
       </c>
       <c r="BQ3">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="BR3">
-        <v>23</v>
-      </c>
-      <c r="BS3">
-        <v>150</v>
-      </c>
-      <c r="BT3">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="AE3:BG3 BS3:XFD3 A3:AA3">
-    <cfRule type="expression" dxfId="6" priority="18" stopIfTrue="1">
+  <conditionalFormatting sqref="AC3:BE3 BQ3:XFD3 A3:Y3">
+    <cfRule type="expression" dxfId="6" priority="20" stopIfTrue="1">
       <formula>A3&lt;&gt;A2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y3">
-    <cfRule type="cellIs" dxfId="5" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="17" operator="lessThan">
       <formula>X2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:Y2">
-    <cfRule type="expression" dxfId="4" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="15" stopIfTrue="1">
       <formula>X2&lt;&gt;X1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE3">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
-      <formula>AD3</formula>
+  <conditionalFormatting sqref="AC3">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="lessThan">
+      <formula>AB3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE2">
+  <conditionalFormatting sqref="BQ2:BR2">
     <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
-      <formula>AE2&lt;&gt;AE1</formula>
+      <formula>BQ2&lt;&gt;BQ1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE2">
+  <conditionalFormatting sqref="AC2">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
-      <formula>AD2</formula>
+      <formula>AB2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BS2:BT2">
+  <conditionalFormatting sqref="AC2">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
-      <formula>BS2&lt;&gt;BS1</formula>
+      <formula>AC2&lt;&gt;AC1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Mother of all bodges to enable home to be disconnected properly
</commit_message>
<xml_diff>
--- a/Inputs/InputSchedule.xlsx
+++ b/Inputs/InputSchedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/ah17992_bristol_ac_uk/Documents/DP5/Shared/DP5_modelling/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{57505528-C0AC-AF43-B518-BDF5D0845882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{046B966E-C5B5-4560-B7A1-C3A92403E256}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{57505528-C0AC-AF43-B518-BDF5D0845882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3FA1386-6903-4AC1-AD1C-32592FA423BE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -279,13 +279,13 @@
     <t>London, UK, HA5 5SG</t>
   </si>
   <si>
-    <t>Electric</t>
-  </si>
-  <si>
-    <t>ASHP</t>
-  </si>
-  <si>
-    <t>GSHP</t>
+    <t>ICE</t>
+  </si>
+  <si>
+    <t>Fixed22Tariff.csv</t>
+  </si>
+  <si>
+    <t>Carbon</t>
   </si>
 </sst>
 </file>
@@ -856,124 +856,7 @@
     <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -1310,8 +1193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BR5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="AM11" sqref="AM11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1668,7 +1551,7 @@
         <v>44</v>
       </c>
       <c r="AF2" s="8" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="AG2" s="8" t="s">
         <v>56</v>
@@ -1684,7 +1567,7 @@
         <v>0.8</v>
       </c>
       <c r="AL2" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM2" s="10"/>
       <c r="AN2" s="8">
@@ -1779,10 +1662,10 @@
     </row>
     <row r="3" spans="1:70" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>49</v>
@@ -1821,7 +1704,7 @@
       </c>
       <c r="P3" s="10"/>
       <c r="Q3" s="8" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="R3" s="8" t="s">
         <v>43</v>
@@ -1869,7 +1752,7 @@
       </c>
       <c r="AH3" s="10"/>
       <c r="AI3" s="8" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="AJ3" s="8">
         <v>9</v>
@@ -1878,11 +1761,11 @@
         <v>0.8</v>
       </c>
       <c r="AL3" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM3" s="10"/>
       <c r="AN3" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO3" s="8">
         <v>5</v>
@@ -1973,10 +1856,10 @@
     </row>
     <row r="4" spans="1:70" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>49</v>
@@ -1999,7 +1882,7 @@
         <v>2437.5</v>
       </c>
       <c r="K4" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4" s="8">
         <v>0.15</v>
@@ -2015,7 +1898,7 @@
       </c>
       <c r="P4" s="10"/>
       <c r="Q4" s="8" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="R4" s="8" t="s">
         <v>43</v>
@@ -2063,7 +1946,7 @@
       </c>
       <c r="AH4" s="10"/>
       <c r="AI4" s="8" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="AJ4" s="8">
         <v>9</v>
@@ -2072,11 +1955,11 @@
         <v>0.8</v>
       </c>
       <c r="AL4" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM4" s="10"/>
       <c r="AN4" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO4" s="8">
         <v>5</v>
@@ -2167,10 +2050,10 @@
     </row>
     <row r="5" spans="1:70" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>49</v>
@@ -2209,7 +2092,7 @@
       </c>
       <c r="P5" s="10"/>
       <c r="Q5" s="8" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>43</v>
@@ -2253,11 +2136,11 @@
         <v>45</v>
       </c>
       <c r="AG5" s="8" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="AH5" s="10"/>
       <c r="AI5" s="8" t="s">
-        <v>84</v>
+        <v>46</v>
       </c>
       <c r="AJ5" s="8">
         <v>9</v>
@@ -2266,11 +2149,11 @@
         <v>0.8</v>
       </c>
       <c r="AL5" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM5" s="10"/>
       <c r="AN5" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO5" s="8">
         <v>5</v>
@@ -2361,94 +2244,19 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="Y2:AB2">
-    <cfRule type="cellIs" dxfId="17" priority="31" operator="lessThan">
+  <conditionalFormatting sqref="Y2:AC5">
+    <cfRule type="cellIs" dxfId="2" priority="31" operator="lessThan">
       <formula>X2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X2:Y2">
-    <cfRule type="expression" dxfId="16" priority="29" stopIfTrue="1">
+  <conditionalFormatting sqref="BQ2:BR4 X2:AC4">
+    <cfRule type="expression" dxfId="1" priority="29" stopIfTrue="1">
       <formula>X2&lt;&gt;X1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BQ2:BR2">
-    <cfRule type="expression" dxfId="15" priority="17" stopIfTrue="1">
-      <formula>BQ2&lt;&gt;BQ1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC2:AC5">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="lessThan">
-      <formula>AB2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC2:AC5">
-    <cfRule type="expression" dxfId="13" priority="15" stopIfTrue="1">
-      <formula>AC2&lt;&gt;AC1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z2:AB2">
-    <cfRule type="expression" dxfId="12" priority="13" stopIfTrue="1">
-      <formula>Z2&lt;&gt;Z1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:AB3">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="lessThan">
-      <formula>X3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X3:Y3">
-    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
-      <formula>X3&lt;&gt;X2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BQ3:BR3">
-    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
-      <formula>BQ3&lt;&gt;BQ2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z3:AB3">
-    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
-      <formula>Z3&lt;&gt;Z2</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y4:AB4">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
-      <formula>X4</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X4:Y4">
-    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
-      <formula>X4&lt;&gt;X3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BQ4:BR4">
-    <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
-      <formula>BQ4&lt;&gt;BQ3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z4:AB4">
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
-      <formula>Z4&lt;&gt;Z3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y5:AB5">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
-      <formula>X5</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X5:Y5">
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
-      <formula>X5&lt;&gt;X4</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BQ5:BR5">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
-      <formula>BQ5&lt;&gt;BQ4</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z5:AB5">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
-      <formula>Z5&lt;&gt;Z4</formula>
+  <conditionalFormatting sqref="BQ5:BR5 X5:AC5">
+    <cfRule type="expression" dxfId="0" priority="33" stopIfTrue="1">
+      <formula>X5&lt;&gt;X3</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Extra plotting and some interesting inputs
</commit_message>
<xml_diff>
--- a/Inputs/InputSchedule.xlsx
+++ b/Inputs/InputSchedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/ah17992_bristol_ac_uk/Documents/DP5/Shared/DP5_modelling/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{57505528-C0AC-AF43-B518-BDF5D0845882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3FA1386-6903-4AC1-AD1C-32592FA423BE}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{57505528-C0AC-AF43-B518-BDF5D0845882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0FB4A31-5C6D-4FE4-8B3E-8D69E086F444}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="86">
   <si>
     <t>Case</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>Carbon</t>
+  </si>
+  <si>
+    <t>Home</t>
   </si>
 </sst>
 </file>
@@ -1194,7 +1197,7 @@
   <dimension ref="A1:BR5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1856,10 +1859,10 @@
     </row>
     <row r="4" spans="1:70" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>49</v>
@@ -1898,7 +1901,7 @@
       </c>
       <c r="P4" s="10"/>
       <c r="Q4" s="8" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="R4" s="8" t="s">
         <v>43</v>
@@ -1939,7 +1942,7 @@
         <v>44</v>
       </c>
       <c r="AF4" s="8" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="AG4" s="8" t="s">
         <v>56</v>
@@ -1955,7 +1958,7 @@
         <v>0.8</v>
       </c>
       <c r="AL4" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM4" s="10"/>
       <c r="AN4" s="8">

</xml_diff>

<commit_message>
carbon journey cost added
</commit_message>
<xml_diff>
--- a/Inputs/InputSchedule.xlsx
+++ b/Inputs/InputSchedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/ah17992_bristol_ac_uk/Documents/DP5/Shared/DP5_modelling/Inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yazzadsukhia/Desktop/DP5_new_mod/DP5_modelling/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{57505528-C0AC-AF43-B518-BDF5D0845882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0FB4A31-5C6D-4FE4-8B3E-8D69E086F444}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C17C077-0C13-774F-910D-854AB1655B69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11420" yWindow="1740" windowWidth="24420" windowHeight="14640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InputSchedule" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="87">
   <si>
     <t>Case</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>Home</t>
+  </si>
+  <si>
+    <t>Carbon Kg per litre Fuel</t>
   </si>
 </sst>
 </file>
@@ -1194,70 +1197,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BR5"/>
+  <dimension ref="A1:BS5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="BU4" sqref="BU4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
     <col min="13" max="15" width="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="17" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="20.28515625" customWidth="1"/>
-    <col min="30" max="30" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="6.28515625" customWidth="1"/>
-    <col min="34" max="34" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.33203125" customWidth="1"/>
+    <col min="30" max="30" width="3.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.33203125" customWidth="1"/>
+    <col min="34" max="34" width="3.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="3.6640625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="4" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="42" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="48" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="3.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="42" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="3.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="48" width="3.6640625" bestFit="1" customWidth="1"/>
     <col min="49" max="50" width="5" bestFit="1" customWidth="1"/>
-    <col min="51" max="52" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="3.6640625" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="4" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="3.6640625" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="4" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="5" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="61" max="65" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="3.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="61" max="65" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="5.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" s="4" customFormat="1" ht="117.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:71" s="4" customFormat="1" ht="118" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>47</v>
       </c>
@@ -1468,8 +1472,11 @@
       <c r="BR1" s="4" t="s">
         <v>74</v>
       </c>
+      <c r="BS1" s="4" t="s">
+        <v>86</v>
+      </c>
     </row>
-    <row r="2" spans="1:70" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:71" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1662,8 +1669,11 @@
       <c r="BR2" s="8">
         <v>50</v>
       </c>
+      <c r="BS2" s="8">
+        <v>2.31</v>
+      </c>
     </row>
-    <row r="3" spans="1:70" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:71" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1856,8 +1866,11 @@
       <c r="BR3" s="8">
         <v>50</v>
       </c>
+      <c r="BS3" s="8">
+        <v>2.31</v>
+      </c>
     </row>
-    <row r="4" spans="1:70" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:71" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -2050,8 +2063,11 @@
       <c r="BR4" s="8">
         <v>50</v>
       </c>
+      <c r="BS4" s="8">
+        <v>2.31</v>
+      </c>
     </row>
-    <row r="5" spans="1:70" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:71" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>2</v>
       </c>
@@ -2243,6 +2259,9 @@
       </c>
       <c r="BR5" s="8">
         <v>50</v>
+      </c>
+      <c r="BS5" s="8">
+        <v>2.31</v>
       </c>
     </row>
   </sheetData>
@@ -2252,7 +2271,7 @@
       <formula>X2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BQ2:BR4 X2:AC4">
+  <conditionalFormatting sqref="BQ2:BR4 X2:AC4 BS2:BS5">
     <cfRule type="expression" dxfId="1" priority="29" stopIfTrue="1">
       <formula>X2&lt;&gt;X1</formula>
     </cfRule>

</xml_diff>